<commit_message>
I rectified my code and change the sleep time to 1000
</commit_message>
<xml_diff>
--- a/my.xlsx
+++ b/my.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19920" windowHeight="8400"/>
+    <workbookView windowWidth="19890" windowHeight="7980"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4">
   <si>
     <t>Monsoon</t>
   </si>
@@ -26,6 +26,9 @@
   </si>
   <si>
     <t>Training</t>
+  </si>
+  <si>
+    <t>By Shubham Sir</t>
   </si>
 </sst>
 </file>
@@ -400,11 +403,11 @@
         </a:custGeom>
         <a:gradFill rotWithShape="0">
           <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="BBD5F0"/>
+            </a:gs>
             <a:gs pos="100000">
               <a:srgbClr val="9CBEE0"/>
-            </a:gs>
-            <a:gs pos="0">
-              <a:srgbClr val="BBD5F0"/>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
@@ -428,13 +431,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelRow="3"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
@@ -451,8 +454,13 @@
         <v>2</v>
       </c>
     </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511111111111111" footer="0.511111111111111"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.510416666666667" footer="0.510416666666667"/>
   <pageSetup paperSize="256" fitToWidth="0" fitToHeight="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="600" verticalDpi="600"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
@@ -469,7 +477,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75"/>
   <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511111111111111" footer="0.511111111111111"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.510416666666667" footer="0.510416666666667"/>
   <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait" useFirstPageNumber="1" errors="NA" horizontalDpi="600" verticalDpi="600"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
@@ -486,7 +494,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75"/>
   <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511111111111111" footer="0.511111111111111"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.510416666666667" footer="0.510416666666667"/>
   <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait" useFirstPageNumber="1" errors="NA" horizontalDpi="600" verticalDpi="600"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>

</xml_diff>